<commit_message>
Line - Get line full info returns markerIcon of stations
</commit_message>
<xml_diff>
--- a/data_sheets/madrid.xlsx
+++ b/data_sheets/madrid.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B8888A-5C1F-49A9-AAEE-366D62EE876E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604F6347-8717-41E6-99E3-42B5402D1C83}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,10 +445,10 @@
         <v>1919</v>
       </c>
       <c r="D2">
+        <v>-3.7056496999999999</v>
+      </c>
+      <c r="E2">
         <v>40.417017700000002</v>
-      </c>
-      <c r="E2">
-        <v>-3.7056496999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -459,10 +459,10 @@
         <v>1924</v>
       </c>
       <c r="D3">
+        <v>-3.7026070999999998</v>
+      </c>
+      <c r="E3">
         <v>40.416827099999999</v>
-      </c>
-      <c r="E3">
-        <v>-3.7026070999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -473,10 +473,10 @@
         <v>1919</v>
       </c>
       <c r="D4">
+        <v>-3.7037949000000001</v>
+      </c>
+      <c r="E4">
         <v>40.419856500000002</v>
-      </c>
-      <c r="E4">
-        <v>-3.7037949000000001</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4DC3D7-5FDB-4774-84FD-C11306A4809B}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>